<commit_message>
Agregando todos los archivos del proyecto
</commit_message>
<xml_diff>
--- a/public/inscripciones.xlsx
+++ b/public/inscripciones.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Nombre</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>15:00</t>
+  </si>
+  <si>
+    <t>Atletismo</t>
+  </si>
+  <si>
+    <t>2024-11-03</t>
   </si>
 </sst>
 </file>
@@ -426,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="30" customWidth="1"/>
@@ -486,6 +492,23 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>